<commit_message>
Refactor code structure and remove redundant sections for improved readability and maintainability; monthly test added
</commit_message>
<xml_diff>
--- a/Homeworks/G2028A2_TL_2025秋.xlsx
+++ b/Homeworks/G2028A2_TL_2025秋.xlsx
@@ -2,13 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="20752" windowHeight="10267" tabRatio="805" activeTab="1"/>
+    <workbookView windowWidth="20752" windowHeight="10267" tabRatio="805" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="11" r:id="rId1"/>
     <sheet name="Week 2" sheetId="12" r:id="rId2"/>
+    <sheet name="Week 3" sheetId="13" r:id="rId3"/>
+    <sheet name="Week 4" sheetId="14" r:id="rId4"/>
+    <sheet name="Week 5" sheetId="15" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="61">
   <si>
     <t>Teacher:</t>
   </si>
@@ -182,6 +185,39 @@
   </si>
   <si>
     <t>chloe</t>
+  </si>
+  <si>
+    <t>梁驭恩</t>
+  </si>
+  <si>
+    <t>A-</t>
+  </si>
+  <si>
+    <t>A+</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C-</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>苏麦嘉</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1342,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:S27"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -2082,11 +2118,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2248,7 +2284,9 @@
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
+      <c r="R6" s="10">
+        <v>99</v>
+      </c>
     </row>
     <row r="7" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
       <c r="A7" s="11">
@@ -2282,7 +2320,9 @@
       </c>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
+      <c r="R7" s="13">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" ht="15" customHeight="1" spans="1:18">
       <c r="A8" s="7">
@@ -2314,7 +2354,9 @@
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
+      <c r="R8" s="10">
+        <v>99</v>
+      </c>
     </row>
     <row r="9" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
       <c r="A9" s="11">
@@ -2348,7 +2390,9 @@
       </c>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
+      <c r="R9" s="13">
+        <v>85</v>
+      </c>
     </row>
     <row r="10" ht="15" customHeight="1" spans="1:18">
       <c r="A10" s="7">
@@ -2382,7 +2426,9 @@
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
+      <c r="R10" s="10">
+        <v>96</v>
+      </c>
     </row>
     <row r="11" s="1" customFormat="1" ht="16" customHeight="1" spans="1:19">
       <c r="A11" s="11">
@@ -2453,7 +2499,9 @@
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
+      <c r="R12" s="10">
+        <v>98</v>
+      </c>
     </row>
     <row r="13" s="1" customFormat="1" ht="17" customHeight="1" spans="1:18">
       <c r="A13" s="11">
@@ -2487,7 +2535,9 @@
       </c>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
+      <c r="R13" s="13">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" ht="16" customHeight="1" spans="1:18">
       <c r="A14" s="7">
@@ -2519,7 +2569,9 @@
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
+      <c r="R14" s="10">
+        <v>100</v>
+      </c>
     </row>
     <row r="15" ht="16" customHeight="1" spans="1:18">
       <c r="A15" s="11">
@@ -2553,7 +2605,9 @@
       </c>
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
+      <c r="R15" s="13">
+        <v>86</v>
+      </c>
     </row>
     <row r="16" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
       <c r="A16" s="7">
@@ -2649,7 +2703,9 @@
       </c>
       <c r="P18" s="16"/>
       <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
+      <c r="R18" s="16">
+        <v>93</v>
+      </c>
     </row>
     <row r="19" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
       <c r="A19" s="11">
@@ -2683,7 +2739,9 @@
       </c>
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
+      <c r="R19" s="13">
+        <v>87</v>
+      </c>
     </row>
     <row r="20" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
       <c r="A20" s="7">
@@ -2712,10 +2770,14 @@
       </c>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
-      <c r="O20" s="16"/>
+      <c r="O20" s="16">
+        <v>92</v>
+      </c>
       <c r="P20" s="16"/>
       <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
+      <c r="R20" s="16">
+        <v>95</v>
+      </c>
     </row>
     <row r="21" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
       <c r="A21" s="11">
@@ -2779,7 +2841,9 @@
       </c>
       <c r="P22" s="16"/>
       <c r="Q22" s="16"/>
-      <c r="R22" s="16"/>
+      <c r="R22" s="16">
+        <v>100</v>
+      </c>
     </row>
     <row r="23" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
       <c r="A23" s="11">
@@ -2818,6 +2882,2478 @@
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+    </row>
+    <row r="25" s="1" customFormat="1" ht="17" customHeight="1" spans="1:18">
+      <c r="A25" s="11">
+        <v>20</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+    </row>
+    <row r="26" ht="17" customHeight="1" spans="1:18">
+      <c r="A26" s="7">
+        <v>21</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+    </row>
+    <row r="27" ht="17" customHeight="1" spans="1:18">
+      <c r="A27" s="11">
+        <v>22</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.298611111111111" footer="0.298611111111111"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A3:S27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="8.6283185840708" customWidth="1"/>
+    <col min="4" max="8" width="5.25663716814159" customWidth="1"/>
+    <col min="9" max="9" width="5.12389380530973" customWidth="1"/>
+    <col min="10" max="11" width="5.25663716814159" customWidth="1"/>
+    <col min="12" max="13" width="5.3716814159292" customWidth="1"/>
+    <col min="14" max="14" width="5.12389380530973" customWidth="1"/>
+    <col min="15" max="17" width="5.3716814159292" customWidth="1"/>
+    <col min="18" max="18" width="5.25663716814159" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" ht="31" customHeight="1" spans="1:17">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+    </row>
+    <row r="4" ht="18" customHeight="1" spans="1:18">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+    </row>
+    <row r="5" ht="38" customHeight="1" spans="1:18">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" ht="17" customHeight="1" spans="1:18">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10">
+        <v>90</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10">
+        <v>97</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10">
+        <v>95</v>
+      </c>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A7" s="11">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13">
+        <v>100</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13">
+        <v>100</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13">
+        <v>84</v>
+      </c>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="1:18">
+      <c r="A8" s="7">
+        <v>3</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10">
+        <v>92</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10">
+        <v>93</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10">
+        <v>92</v>
+      </c>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A9" s="11">
+        <v>4</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13">
+        <v>100</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13">
+        <v>100</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13">
+        <v>100</v>
+      </c>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="1:18">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10">
+        <v>85</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10">
+        <v>100</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10">
+        <v>95</v>
+      </c>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" ht="16" customHeight="1" spans="1:19">
+      <c r="A11" s="11">
+        <v>6</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13">
+        <v>100</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13">
+        <v>97</v>
+      </c>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13">
+        <v>100</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" ht="17" customHeight="1" spans="1:18">
+      <c r="A12" s="7">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10">
+        <v>85</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10">
+        <v>88</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10">
+        <v>92</v>
+      </c>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="17" customHeight="1" spans="1:18">
+      <c r="A13" s="11">
+        <v>8</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13">
+        <v>30</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13">
+        <v>65</v>
+      </c>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" ht="16" customHeight="1" spans="1:18">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10">
+        <v>93</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10">
+        <v>99</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10">
+        <v>90</v>
+      </c>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" ht="16" customHeight="1" spans="1:18">
+      <c r="A15" s="11">
+        <v>10</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13">
+        <v>80</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13">
+        <v>93</v>
+      </c>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13">
+        <v>84</v>
+      </c>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A16" s="7">
+        <v>11</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+    </row>
+    <row r="17" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A17" s="11">
+        <v>12</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+    </row>
+    <row r="18" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A18" s="7">
+        <v>13</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16">
+        <v>100</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16">
+        <v>97</v>
+      </c>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16">
+        <v>97</v>
+      </c>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A19" s="11">
+        <v>14</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13">
+        <v>85</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13">
+        <v>92</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13">
+        <v>92</v>
+      </c>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A20" s="7">
+        <v>15</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16">
+        <v>100</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16">
+        <v>95</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+    </row>
+    <row r="21" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A21" s="11">
+        <v>16</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13">
+        <v>50</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13">
+        <v>90</v>
+      </c>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13">
+        <v>80</v>
+      </c>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+    </row>
+    <row r="22" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A22" s="7">
+        <v>17</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16">
+        <v>98</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16">
+        <v>100</v>
+      </c>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16">
+        <v>100</v>
+      </c>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A23" s="11">
+        <v>18</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13">
+        <v>50</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13">
+        <v>80</v>
+      </c>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A24" s="7">
+        <v>19</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+    </row>
+    <row r="25" s="1" customFormat="1" ht="17" customHeight="1" spans="1:18">
+      <c r="A25" s="11">
+        <v>20</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+    </row>
+    <row r="26" ht="17" customHeight="1" spans="1:18">
+      <c r="A26" s="7">
+        <v>21</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+    </row>
+    <row r="27" ht="17" customHeight="1" spans="1:18">
+      <c r="A27" s="11">
+        <v>22</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.298611111111111" footer="0.298611111111111"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A3:S27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="8.6283185840708" customWidth="1"/>
+    <col min="4" max="8" width="5.25663716814159" customWidth="1"/>
+    <col min="9" max="9" width="5.12389380530973" customWidth="1"/>
+    <col min="10" max="11" width="5.25663716814159" customWidth="1"/>
+    <col min="12" max="13" width="5.3716814159292" customWidth="1"/>
+    <col min="14" max="14" width="5.12389380530973" customWidth="1"/>
+    <col min="15" max="17" width="5.3716814159292" customWidth="1"/>
+    <col min="18" max="18" width="5.25663716814159" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" ht="31" customHeight="1" spans="1:17">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+    </row>
+    <row r="4" ht="18" customHeight="1" spans="1:18">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+    </row>
+    <row r="5" ht="38" customHeight="1" spans="1:18">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" ht="17" customHeight="1" spans="1:18">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10">
+        <v>86</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10">
+        <v>88</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A7" s="11">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13">
+        <v>94</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13">
+        <v>90</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="1:18">
+      <c r="A8" s="7">
+        <v>3</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10">
+        <v>76</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A9" s="11">
+        <v>4</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13">
+        <v>92</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13">
+        <v>91</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="1:18">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10">
+        <v>87</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10">
+        <v>96</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+    </row>
+    <row r="11" s="1" customFormat="1" ht="16" customHeight="1" spans="1:19">
+      <c r="A11" s="11">
+        <v>6</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13">
+        <v>96</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" ht="17" customHeight="1" spans="1:18">
+      <c r="A12" s="7">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10">
+        <v>70</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10">
+        <v>87</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="17" customHeight="1" spans="1:18">
+      <c r="A13" s="11">
+        <v>8</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13">
+        <v>10</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13">
+        <v>15</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+    </row>
+    <row r="14" ht="16" customHeight="1" spans="1:18">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10">
+        <v>95</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" ht="16" customHeight="1" spans="1:18">
+      <c r="A15" s="11">
+        <v>10</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13">
+        <v>82</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13">
+        <v>84</v>
+      </c>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A16" s="7">
+        <v>11</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+    </row>
+    <row r="17" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A17" s="11">
+        <v>12</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+    </row>
+    <row r="18" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A18" s="7">
+        <v>13</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16">
+        <v>96</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16">
+        <v>95</v>
+      </c>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A19" s="11">
+        <v>14</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13">
+        <v>78</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13">
+        <v>72</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A20" s="7">
+        <v>15</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16">
+        <v>94</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16">
+        <v>100</v>
+      </c>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A21" s="11">
+        <v>16</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13">
+        <v>60</v>
+      </c>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+    </row>
+    <row r="22" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A22" s="7">
+        <v>17</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16">
+        <v>96</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16">
+        <v>49</v>
+      </c>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A23" s="11">
+        <v>18</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13">
+        <v>82</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13">
+        <v>80</v>
+      </c>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A24" s="7">
+        <v>19</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16">
+        <v>95</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16">
+        <v>99</v>
+      </c>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" s="1" customFormat="1" ht="17" customHeight="1" spans="1:18">
+      <c r="A25" s="11">
+        <v>20</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+    </row>
+    <row r="26" ht="17" customHeight="1" spans="1:18">
+      <c r="A26" s="7">
+        <v>21</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+    </row>
+    <row r="27" ht="17" customHeight="1" spans="1:18">
+      <c r="A27" s="11">
+        <v>22</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.298611111111111" footer="0.298611111111111"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A3:S27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="8.6283185840708" customWidth="1"/>
+    <col min="4" max="8" width="5.25663716814159" customWidth="1"/>
+    <col min="9" max="9" width="5.12389380530973" customWidth="1"/>
+    <col min="10" max="11" width="5.25663716814159" customWidth="1"/>
+    <col min="12" max="13" width="5.3716814159292" customWidth="1"/>
+    <col min="14" max="14" width="5.12389380530973" customWidth="1"/>
+    <col min="15" max="17" width="5.3716814159292" customWidth="1"/>
+    <col min="18" max="18" width="5.25663716814159" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" ht="31" customHeight="1" spans="1:17">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+    </row>
+    <row r="4" ht="18" customHeight="1" spans="1:18">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+    </row>
+    <row r="5" ht="38" customHeight="1" spans="1:18">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" ht="17" customHeight="1" spans="1:18">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A7" s="11">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13">
+        <v>4</v>
+      </c>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="1:18">
+      <c r="A8" s="7">
+        <v>3</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A9" s="11">
+        <v>4</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="1:18">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+    </row>
+    <row r="11" s="1" customFormat="1" ht="16" customHeight="1" spans="1:19">
+      <c r="A11" s="11">
+        <v>6</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" ht="17" customHeight="1" spans="1:18">
+      <c r="A12" s="7">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+    </row>
+    <row r="13" s="1" customFormat="1" ht="17" customHeight="1" spans="1:18">
+      <c r="A13" s="11">
+        <v>8</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+    </row>
+    <row r="14" ht="16" customHeight="1" spans="1:18">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10">
+        <v>2</v>
+      </c>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+    </row>
+    <row r="15" ht="16" customHeight="1" spans="1:18">
+      <c r="A15" s="11">
+        <v>10</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+    </row>
+    <row r="16" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A16" s="7">
+        <v>11</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+    </row>
+    <row r="17" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A17" s="11">
+        <v>12</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+    </row>
+    <row r="18" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A18" s="7">
+        <v>13</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="16"/>
+    </row>
+    <row r="19" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A19" s="11">
+        <v>14</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+    </row>
+    <row r="20" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A20" s="7">
+        <v>15</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+    </row>
+    <row r="21" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A21" s="11">
+        <v>16</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+    </row>
+    <row r="22" s="1" customFormat="1" ht="16" customHeight="1" spans="1:18">
+      <c r="A22" s="7">
+        <v>17</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+    </row>
+    <row r="23" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A23" s="11">
+        <v>18</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="17"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13">
+        <v>3</v>
+      </c>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+    </row>
+    <row r="24" s="1" customFormat="1" ht="15" customHeight="1" spans="1:18">
+      <c r="A24" s="7">
+        <v>19</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16">
+        <v>5</v>
+      </c>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>

</xml_diff>